<commit_message>
add data check module Signed-off-by: love19862003 <love19862003@163.com>
</commit_message>
<xml_diff>
--- a/bin/setting.xlsx
+++ b/bin/setting.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>包名。Package</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,10 +92,6 @@
   </si>
   <si>
     <t>role</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>role1.xlsx</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -113,6 +109,22 @@
       </rPr>
       <t>ob,level,sub</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>check.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>check</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>role.xlsx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monster.xlsx</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -557,9 +569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
   <cols>
@@ -570,18 +580,18 @@
   <sheetData>
     <row r="1" spans="1:256" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:256" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -1253,7 +1263,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1264,8 +1274,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>

</xml_diff>